<commit_message>
add C# delegate code
</commit_message>
<xml_diff>
--- a/Backend/2. C#/C#笔记.xlsx
+++ b/Backend/2. C#/C#笔记.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janss\Desktop\Full-stack\Backend\2. C#\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3509B5C2-481A-4130-A65F-5FE8173995A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AB499F-16F8-4AA9-97B7-C07A0CD2436F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{FDF50CD9-36D8-4159-AC2D-F632DE44E8E7}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FDF50CD9-36D8-4159-AC2D-F632DE44E8E7}"/>
   </bookViews>
   <sheets>
     <sheet name="C#导航栏" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="405">
   <si>
     <t>日志和监控
 使用Serilog或NLog
@@ -1176,32 +1176,6 @@
     <t>2. 委托是类型还是成员？如何声明委托？方法申明委托有哪些格式要求呢？如何创建委托对象并赋值?如何从委托添加或者减少方法？</t>
   </si>
   <si>
-    <r>
-      <t>从委托通过 += 添加或者 -= 减少方法（注意：通过这种方法实际上是</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>创建了一个新的对象</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
     <t>3. 如何调用委托？分无返回值、有值类型参数、有引用参数</t>
   </si>
   <si>
@@ -1696,7 +1670,72 @@
     <t>5. 泛型方法——了解如何声明泛型方法、调用泛型方法</t>
   </si>
   <si>
-    <t>6. 扩展方法和泛型类</t>
+    <t>2. 必须是静态类的成员</t>
+  </si>
+  <si>
+    <t>3. 第一个参数类型中必须要有this关键字，后面是扩展的泛型类的名字</t>
+  </si>
+  <si>
+    <t>1. 类名必须声明为static</t>
+  </si>
+  <si>
+    <t>6. 扩展方法使用的场景是什么？扩展方法在泛型类上的语法是什么？</t>
+  </si>
+  <si>
+    <t>7. 泛型结构 ——  与泛型类一样</t>
+  </si>
+  <si>
+    <t>8. 委托泛型</t>
+  </si>
+  <si>
+    <r>
+      <t>从委托通过 += 添加或者 -= 减少方法（很少用）（注意：通过这种方法实际上是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>创建了一个新的对象</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <t>1. function声明的语法是什么？function在哪里声明？</t>
+  </si>
+  <si>
+    <t>2. function里的变量叫什么？和在类里定义的变量有什么区别？function里变量申明的语法是什么？</t>
+  </si>
+  <si>
+    <t>3. C#中var和js中var的区别？简述C#中var的作用</t>
+  </si>
+  <si>
+    <t>4. 什么是常量？申明的语法规则是什么？在function中和在class中有什么区别</t>
+  </si>
+  <si>
+    <t>5. 方法如何在内部调用和在外部调用？</t>
+  </si>
+  <si>
+    <t>6. 什么是实参，什么是形参？形参分为哪几种类型？请简述堆栈图</t>
+  </si>
+  <si>
+    <t>7. 详细描述什么是参数数组？声明的语法规则是什么？有哪些注意事项？了解可选参数的声明顺序</t>
+  </si>
+  <si>
+    <t>8. 了解方法重载. 简述哪些地方不同可以方法重载</t>
   </si>
 </sst>
 </file>
@@ -2073,7 +2112,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2252,13 +2291,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2267,13 +2300,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2284,9 +2320,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -29786,7 +29819,19 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>方法二（推荐）</a:t>
+            <a:t>方法二（推荐）更加建议用</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>lambda</a:t>
           </a:r>
           <a:endParaRPr lang="en-AU" altLang="zh-CN" sz="1100" baseline="0">
             <a:solidFill>
@@ -31129,13 +31174,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>208</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -31422,13 +31467,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>162</xdr:row>
+      <xdr:row>210</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -31785,13 +31830,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>162</xdr:row>
+      <xdr:row>210</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -32101,13 +32146,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>216</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>183</xdr:row>
+      <xdr:row>231</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -32394,13 +32439,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>216</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>186</xdr:row>
+      <xdr:row>234</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -32720,13 +32765,13 @@
     <xdr:from>
       <xdr:col>33</xdr:col>
       <xdr:colOff>398369</xdr:colOff>
-      <xdr:row>186</xdr:row>
+      <xdr:row>234</xdr:row>
       <xdr:rowOff>160804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>593911</xdr:colOff>
-      <xdr:row>190</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>160803</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -32788,13 +32833,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>13607</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>216</xdr:row>
       <xdr:rowOff>136070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>508907</xdr:colOff>
-      <xdr:row>186</xdr:row>
+      <xdr:row>234</xdr:row>
       <xdr:rowOff>123265</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -33177,13 +33222,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>408214</xdr:colOff>
-      <xdr:row>186</xdr:row>
+      <xdr:row>234</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>610960</xdr:colOff>
-      <xdr:row>190</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>163285</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -33245,13 +33290,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>375958</xdr:colOff>
-      <xdr:row>186</xdr:row>
+      <xdr:row>234</xdr:row>
       <xdr:rowOff>138393</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>190</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>138392</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -33313,13 +33358,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>191</xdr:row>
+      <xdr:row>239</xdr:row>
       <xdr:rowOff>123265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>392206</xdr:colOff>
-      <xdr:row>205</xdr:row>
+      <xdr:row>253</xdr:row>
       <xdr:rowOff>11207</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -33567,13 +33612,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>112059</xdr:colOff>
-      <xdr:row>191</xdr:row>
+      <xdr:row>239</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>2241</xdr:colOff>
-      <xdr:row>208</xdr:row>
+      <xdr:row>256</xdr:row>
       <xdr:rowOff>83483</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -33895,13 +33940,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>168089</xdr:colOff>
-      <xdr:row>191</xdr:row>
+      <xdr:row>239</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>110940</xdr:colOff>
-      <xdr:row>204</xdr:row>
+      <xdr:row>252</xdr:row>
       <xdr:rowOff>11206</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -35471,6 +35516,486 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>        functionA.PrintDatas(20, new int[] { 1, 2, 4 });</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>}</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="TextBox 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ECAB4BE-E4C5-4D61-AC56-87B3FCC0C5DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6429375" y="25384124"/>
+          <a:ext cx="4267200" cy="3305175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>class Method&lt;T&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>{</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    static private T[] arr = new T[10];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    static private int i;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    internal T[] Array =&gt; arr;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    internal int Length =&gt; arr.Length;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AU" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    public void addArr(T a)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        if(i &gt;= arr.Length)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            Console.WriteLine("Array is full");</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        arr[i] = a;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        Console.WriteLine($"Added element at position {i} :{arr[i]}");</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        i++;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>}</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="TextBox 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF600E46-B19C-4D53-B8B2-7C01A5DA115B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11887200" y="25527000"/>
+          <a:ext cx="4267200" cy="1866900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>static class ExtendedMethods</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>{</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    public static T GetElement&lt;T&gt;(this Method&lt;T&gt; method, int index)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        if (index &lt; 0 || index &gt;= method.Length)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            throw new IndexOutOfRangeException();</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>        return method.Array[index];</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -35922,7 +36447,7 @@
     </row>
     <row r="7" spans="2:22">
       <c r="B7" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H7" s="55"/>
       <c r="I7" s="55"/>
@@ -36303,8 +36828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E73D4A-172B-4D97-AD02-0D0188B38C02}">
   <dimension ref="B2:AM320"/>
   <sheetViews>
-    <sheetView topLeftCell="A271" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L129" sqref="L129"/>
+    <sheetView topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H32:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36797,38 +37322,38 @@
     </row>
     <row r="237" spans="2:3">
       <c r="B237" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="239" spans="2:3">
       <c r="C239" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="241" spans="2:4">
       <c r="D241" s="49" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="243" spans="2:4">
       <c r="D243" s="49" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="245" spans="2:4">
       <c r="D245" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="247" spans="2:4">
       <c r="C247" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="248" spans="2:4" s="2" customFormat="1"/>
     <row r="249" spans="2:4">
       <c r="B249" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="251" spans="2:4">
@@ -36843,32 +37368,32 @@
     </row>
     <row r="268" spans="3:3">
       <c r="C268" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="270" spans="3:3">
       <c r="C270" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="272" spans="3:3">
       <c r="C272" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="274" spans="3:3">
       <c r="C274" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="309" spans="2:19">
       <c r="O309" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="310" spans="2:19">
       <c r="B310" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="311" spans="2:19">
@@ -36879,7 +37404,7 @@
     </row>
     <row r="312" spans="2:19">
       <c r="C312" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="314" spans="2:19">
@@ -36930,8 +37455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A75EC0-F63A-4F3C-A639-656A73033C72}">
   <dimension ref="B2:X249"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U198" sqref="U198:U205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -37255,7 +37780,7 @@
     </row>
     <row r="48" spans="3:7">
       <c r="D48" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -37280,7 +37805,7 @@
     </row>
     <row r="72" spans="3:11">
       <c r="C72" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="77" spans="3:11">
@@ -37427,7 +37952,7 @@
     </row>
     <row r="115" spans="4:24">
       <c r="R115" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="116" spans="4:24">
@@ -37691,7 +38216,7 @@
     </row>
     <row r="157" spans="3:23">
       <c r="D157" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="159" spans="3:23">
@@ -37721,52 +38246,90 @@
     </row>
     <row r="192" spans="3:3">
       <c r="C192" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="194" spans="3:21">
+      <c r="D194" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="194" spans="3:4">
-      <c r="D194" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="197" spans="3:4">
+    <row r="197" spans="3:21">
       <c r="C197" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="199" spans="3:4">
+    <row r="198" spans="3:21">
+      <c r="U198" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="199" spans="3:21">
       <c r="D199" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="U199" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="200" spans="3:21">
+      <c r="U200" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="201" spans="3:21">
+      <c r="U201" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="202" spans="3:21">
+      <c r="U202" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="203" spans="3:21">
+      <c r="U203" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="204" spans="3:21">
+      <c r="U204" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="205" spans="3:21">
+      <c r="U205" s="1" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="229" spans="2:4">
       <c r="B229" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="231" spans="2:4">
       <c r="C231" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="233" spans="2:4">
       <c r="D233" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="235" spans="2:4">
       <c r="D235" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="237" spans="2:4">
       <c r="D237" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="239" spans="2:4">
       <c r="C239" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="241" spans="4:6">
@@ -37774,7 +38337,7 @@
         <v>72</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="243" spans="4:6">
@@ -37782,7 +38345,7 @@
         <v>71</v>
       </c>
       <c r="F243" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="245" spans="4:6">
@@ -37790,7 +38353,7 @@
         <v>73</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="247" spans="4:6">
@@ -37798,7 +38361,7 @@
         <v>74</v>
       </c>
       <c r="F247" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="249" spans="4:6">
@@ -37806,7 +38369,7 @@
         <v>75</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -37819,7 +38382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8857E835-7E0E-4F11-9E7E-27875E254D24}">
   <dimension ref="E3:AG183"/>
   <sheetViews>
-    <sheetView topLeftCell="D169" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Y162" sqref="Y162"/>
     </sheetView>
   </sheetViews>
@@ -38168,7 +38731,7 @@
     </row>
     <row r="62" spans="5:26" ht="15.75" thickBot="1">
       <c r="F62" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="V62" s="23"/>
       <c r="W62" s="24"/>
@@ -38222,7 +38785,7 @@
     <row r="91" spans="5:33">
       <c r="AC91" s="20"/>
       <c r="AD91" s="44" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AE91" s="43"/>
       <c r="AF91" s="14"/>
@@ -38322,37 +38885,37 @@
     </row>
     <row r="123" spans="5:6">
       <c r="E123" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="125" spans="5:6">
       <c r="F125" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="127" spans="5:6">
       <c r="F127" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="129" spans="7:7">
       <c r="G129" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="155" spans="7:8">
       <c r="G155" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="157" spans="7:8">
       <c r="H157" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="183" spans="5:5">
       <c r="E183" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -38492,7 +39055,7 @@
     </row>
     <row r="10" spans="1:29">
       <c r="B10" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:29">
@@ -38960,8 +39523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34AB0AF-5F6E-495D-A7A0-8B2ACC54B75F}">
   <dimension ref="D4:AW139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:BE205"/>
+    <sheetView topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39038,38 +39601,38 @@
         <v>282</v>
       </c>
       <c r="P72" s="1" t="s">
-        <v>284</v>
+        <v>396</v>
       </c>
     </row>
     <row r="89" spans="5:20">
       <c r="E89" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="91" spans="5:20">
       <c r="F91" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="94" spans="5:20">
       <c r="G94" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="L94" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="L94" s="1" t="s">
+      <c r="T94" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="T94" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="134" spans="5:49">
       <c r="E134" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="136" spans="5:49">
       <c r="F136" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="139" spans="5:49">
@@ -39097,10 +39660,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D9CD6D-1EAA-4EE6-897F-5DE4D2098EAD}">
-  <dimension ref="I2:AI199"/>
+  <dimension ref="I2:AI247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J126" sqref="J126"/>
+    <sheetView topLeftCell="F197" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J156" sqref="J156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39119,187 +39682,187 @@
     </row>
     <row r="4" spans="9:11">
       <c r="J4" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="9:11">
       <c r="K6" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="21" spans="10:23">
       <c r="K21" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="23" spans="10:23">
       <c r="J23" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="25" spans="10:23">
       <c r="K25" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="27" spans="10:23">
       <c r="J27" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28" spans="10:23">
       <c r="V28" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="10:23">
       <c r="K29" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="10:23">
       <c r="W30" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="31" spans="10:23">
       <c r="L31" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="10:23">
       <c r="L32" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="33" spans="10:12">
       <c r="L33" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="42" spans="10:12">
       <c r="K42" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="46" spans="10:12">
       <c r="J46" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="48" spans="10:12">
       <c r="K48" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="50" spans="11:23">
       <c r="K50" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="52" spans="11:23">
       <c r="K52" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="55" spans="11:23">
       <c r="K55" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="57" spans="11:23">
+      <c r="L57" s="60" t="s">
+        <v>374</v>
+      </c>
+      <c r="M57" s="61" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="57" spans="11:23">
-      <c r="L57" s="61" t="s">
-        <v>375</v>
-      </c>
-      <c r="M57" s="63" t="s">
-        <v>372</v>
-      </c>
-      <c r="N57" s="64"/>
+      <c r="N57" s="62"/>
       <c r="O57" s="59" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="P57" s="59"/>
       <c r="Q57" s="59"/>
       <c r="R57" s="59"/>
       <c r="S57" s="59"/>
       <c r="T57" s="59"/>
-      <c r="U57" s="70" t="s">
-        <v>383</v>
-      </c>
-      <c r="V57" s="70"/>
-      <c r="W57" s="70"/>
+      <c r="U57" s="69" t="s">
+        <v>382</v>
+      </c>
+      <c r="V57" s="69"/>
+      <c r="W57" s="69"/>
     </row>
     <row r="58" spans="11:23">
-      <c r="L58" s="61"/>
-      <c r="M58" s="60" t="s">
+      <c r="L58" s="60"/>
+      <c r="M58" s="63" t="s">
         <v>44</v>
       </c>
       <c r="N58" s="58"/>
-      <c r="O58" s="61" t="s">
-        <v>380</v>
-      </c>
-      <c r="P58" s="68"/>
-      <c r="Q58" s="68"/>
-      <c r="R58" s="68"/>
-      <c r="S58" s="68"/>
-      <c r="T58" s="69"/>
-      <c r="U58" s="70"/>
-      <c r="V58" s="70"/>
-      <c r="W58" s="70"/>
+      <c r="O58" s="60" t="s">
+        <v>379</v>
+      </c>
+      <c r="P58" s="67"/>
+      <c r="Q58" s="67"/>
+      <c r="R58" s="67"/>
+      <c r="S58" s="67"/>
+      <c r="T58" s="68"/>
+      <c r="U58" s="69"/>
+      <c r="V58" s="69"/>
+      <c r="W58" s="69"/>
     </row>
     <row r="59" spans="11:23">
-      <c r="L59" s="61"/>
-      <c r="M59" s="65" t="s">
+      <c r="L59" s="60"/>
+      <c r="M59" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="N59" s="66"/>
-      <c r="O59" s="61" t="s">
-        <v>379</v>
-      </c>
-      <c r="P59" s="68"/>
-      <c r="Q59" s="68"/>
-      <c r="R59" s="68"/>
-      <c r="S59" s="68"/>
-      <c r="T59" s="69"/>
-      <c r="U59" s="70"/>
-      <c r="V59" s="70"/>
-      <c r="W59" s="70"/>
+      <c r="N59" s="65"/>
+      <c r="O59" s="60" t="s">
+        <v>378</v>
+      </c>
+      <c r="P59" s="67"/>
+      <c r="Q59" s="67"/>
+      <c r="R59" s="67"/>
+      <c r="S59" s="67"/>
+      <c r="T59" s="68"/>
+      <c r="U59" s="69"/>
+      <c r="V59" s="69"/>
+      <c r="W59" s="69"/>
     </row>
     <row r="60" spans="11:23">
       <c r="L60" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="M60" s="62" t="s">
-        <v>373</v>
-      </c>
-      <c r="N60" s="62"/>
-      <c r="O60" s="61" t="s">
-        <v>381</v>
-      </c>
-      <c r="P60" s="68"/>
-      <c r="Q60" s="68"/>
-      <c r="R60" s="68"/>
-      <c r="S60" s="68"/>
-      <c r="T60" s="69"/>
+        <v>375</v>
+      </c>
+      <c r="M60" s="66" t="s">
+        <v>372</v>
+      </c>
+      <c r="N60" s="66"/>
+      <c r="O60" s="60" t="s">
+        <v>380</v>
+      </c>
+      <c r="P60" s="67"/>
+      <c r="Q60" s="67"/>
+      <c r="R60" s="67"/>
+      <c r="S60" s="67"/>
+      <c r="T60" s="68"/>
       <c r="U60" s="59" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="V60" s="59"/>
       <c r="W60" s="59"/>
     </row>
     <row r="61" spans="11:23">
       <c r="L61" s="12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M61" s="59" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="N61" s="59"/>
       <c r="O61" s="59" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="P61" s="59"/>
       <c r="Q61" s="59"/>
@@ -39307,588 +39870,578 @@
       <c r="S61" s="59"/>
       <c r="T61" s="59"/>
       <c r="U61" s="59" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="V61" s="59"/>
       <c r="W61" s="59"/>
     </row>
     <row r="62" spans="11:23">
-      <c r="L62" s="71"/>
-      <c r="M62" s="67"/>
-      <c r="N62" s="67"/>
-      <c r="O62" s="67"/>
-      <c r="P62" s="67"/>
-      <c r="Q62" s="67"/>
-      <c r="R62" s="67"/>
-      <c r="S62" s="67"/>
-      <c r="T62" s="67"/>
-      <c r="U62" s="67"/>
-      <c r="V62" s="67"/>
-      <c r="W62" s="67"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+      <c r="V62" s="3"/>
+      <c r="W62" s="3"/>
     </row>
     <row r="63" spans="11:23">
-      <c r="L63" s="71"/>
-      <c r="M63" s="67"/>
-      <c r="N63" s="67"/>
-      <c r="O63" s="67"/>
-      <c r="P63" s="67"/>
-      <c r="Q63" s="67"/>
-      <c r="R63" s="67"/>
-      <c r="S63" s="67"/>
-      <c r="T63" s="67"/>
-      <c r="U63" s="67"/>
-      <c r="V63" s="67"/>
-      <c r="W63" s="67"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="3"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
     </row>
     <row r="64" spans="11:23">
-      <c r="L64" s="71"/>
-      <c r="M64" s="67"/>
-      <c r="N64" s="67"/>
-      <c r="O64" s="67"/>
-      <c r="P64" s="67"/>
-      <c r="Q64" s="67"/>
-      <c r="R64" s="67"/>
-      <c r="S64" s="67"/>
-      <c r="T64" s="67"/>
-      <c r="U64" s="67"/>
-      <c r="V64" s="67"/>
-      <c r="W64" s="67"/>
-    </row>
-    <row r="65" spans="12:23">
-      <c r="L65" s="71"/>
-      <c r="M65" s="67"/>
-      <c r="N65" s="67"/>
-      <c r="O65" s="67"/>
-      <c r="P65" s="67"/>
-      <c r="Q65" s="67"/>
-      <c r="R65" s="67"/>
-      <c r="S65" s="67"/>
-      <c r="T65" s="67"/>
-      <c r="U65" s="67"/>
-      <c r="V65" s="67"/>
-      <c r="W65" s="67"/>
-    </row>
-    <row r="66" spans="12:23">
-      <c r="L66" s="71"/>
-      <c r="M66" s="67"/>
-      <c r="N66" s="67"/>
-      <c r="O66" s="67"/>
-      <c r="P66" s="67"/>
-      <c r="Q66" s="67"/>
-      <c r="R66" s="67"/>
-      <c r="S66" s="67"/>
-      <c r="T66" s="67"/>
-      <c r="U66" s="67"/>
-      <c r="V66" s="67"/>
-      <c r="W66" s="67"/>
-    </row>
-    <row r="67" spans="12:23">
-      <c r="L67" s="71"/>
-      <c r="M67" s="67"/>
-      <c r="N67" s="67"/>
-      <c r="O67" s="67"/>
-      <c r="P67" s="67"/>
-      <c r="Q67" s="67"/>
-      <c r="R67" s="67"/>
-      <c r="S67" s="67"/>
-      <c r="T67" s="67"/>
-      <c r="U67" s="67"/>
-      <c r="V67" s="67"/>
-      <c r="W67" s="67"/>
-    </row>
-    <row r="68" spans="12:23">
-      <c r="L68" s="71"/>
-      <c r="M68" s="67"/>
-      <c r="N68" s="67"/>
-      <c r="O68" s="67"/>
-      <c r="P68" s="67"/>
-      <c r="Q68" s="67"/>
-      <c r="R68" s="67"/>
-      <c r="S68" s="67"/>
-      <c r="T68" s="67"/>
-      <c r="U68" s="67"/>
-      <c r="V68" s="67"/>
-      <c r="W68" s="67"/>
-    </row>
-    <row r="69" spans="12:23">
-      <c r="L69" s="71"/>
-      <c r="M69" s="67"/>
-      <c r="N69" s="67"/>
-      <c r="O69" s="67"/>
-      <c r="P69" s="67"/>
-      <c r="Q69" s="67"/>
-      <c r="R69" s="67"/>
-      <c r="S69" s="67"/>
-      <c r="T69" s="67"/>
-      <c r="U69" s="67"/>
-      <c r="V69" s="67"/>
-      <c r="W69" s="67"/>
-    </row>
-    <row r="70" spans="12:23">
-      <c r="L70" s="71"/>
-      <c r="M70" s="67"/>
-      <c r="N70" s="67"/>
-      <c r="O70" s="67"/>
-      <c r="P70" s="67"/>
-      <c r="Q70" s="67"/>
-      <c r="R70" s="67"/>
-      <c r="S70" s="67"/>
-      <c r="T70" s="67"/>
-      <c r="U70" s="67"/>
-      <c r="V70" s="67"/>
-      <c r="W70" s="67"/>
-    </row>
-    <row r="71" spans="12:23">
-      <c r="L71" s="71"/>
-      <c r="M71" s="67"/>
-      <c r="N71" s="67"/>
-      <c r="O71" s="67"/>
-      <c r="P71" s="67"/>
-      <c r="Q71" s="67"/>
-      <c r="R71" s="67"/>
-      <c r="S71" s="67"/>
-      <c r="T71" s="67"/>
-      <c r="U71" s="67"/>
-      <c r="V71" s="67"/>
-      <c r="W71" s="67"/>
-    </row>
-    <row r="72" spans="12:23">
-      <c r="L72" s="71"/>
-      <c r="M72" s="67"/>
-      <c r="N72" s="67"/>
-      <c r="O72" s="67"/>
-      <c r="P72" s="67"/>
-      <c r="Q72" s="67"/>
-      <c r="R72" s="67"/>
-      <c r="S72" s="67"/>
-      <c r="T72" s="67"/>
-      <c r="U72" s="67"/>
-      <c r="V72" s="67"/>
-      <c r="W72" s="67"/>
-    </row>
-    <row r="73" spans="12:23">
-      <c r="L73" s="71"/>
-      <c r="M73" s="67"/>
-      <c r="N73" s="67"/>
-      <c r="O73" s="67"/>
-      <c r="P73" s="67"/>
-      <c r="Q73" s="67"/>
-      <c r="R73" s="67"/>
-      <c r="S73" s="67"/>
-      <c r="T73" s="67"/>
-      <c r="U73" s="67"/>
-      <c r="V73" s="67"/>
-      <c r="W73" s="67"/>
-    </row>
-    <row r="74" spans="12:23">
-      <c r="L74" s="71"/>
-      <c r="M74" s="67"/>
-      <c r="N74" s="67"/>
-      <c r="O74" s="67"/>
-      <c r="P74" s="67"/>
-      <c r="Q74" s="67"/>
-      <c r="R74" s="67"/>
-      <c r="S74" s="67"/>
-      <c r="T74" s="67"/>
-      <c r="U74" s="67"/>
-      <c r="V74" s="67"/>
-      <c r="W74" s="67"/>
-    </row>
-    <row r="75" spans="12:23">
-      <c r="L75" s="71"/>
-      <c r="M75" s="67"/>
-      <c r="N75" s="67"/>
-      <c r="O75" s="67"/>
-      <c r="P75" s="67"/>
-      <c r="Q75" s="67"/>
-      <c r="R75" s="67"/>
-      <c r="S75" s="67"/>
-      <c r="T75" s="67"/>
-      <c r="U75" s="67"/>
-      <c r="V75" s="67"/>
-      <c r="W75" s="67"/>
-    </row>
-    <row r="76" spans="12:23">
-      <c r="L76" s="71"/>
-      <c r="M76" s="67"/>
-      <c r="N76" s="67"/>
-      <c r="O76" s="67"/>
-      <c r="P76" s="67"/>
-      <c r="Q76" s="67"/>
-      <c r="R76" s="67"/>
-      <c r="S76" s="67"/>
-      <c r="T76" s="67"/>
-      <c r="U76" s="67"/>
-      <c r="V76" s="67"/>
-      <c r="W76" s="67"/>
-    </row>
-    <row r="77" spans="12:23">
-      <c r="L77" s="71"/>
-      <c r="M77" s="67"/>
-      <c r="N77" s="67"/>
-      <c r="O77" s="67"/>
-      <c r="P77" s="67"/>
-      <c r="Q77" s="67"/>
-      <c r="R77" s="67"/>
-      <c r="S77" s="67"/>
-      <c r="T77" s="67"/>
-      <c r="U77" s="67"/>
-      <c r="V77" s="67"/>
-      <c r="W77" s="67"/>
-    </row>
-    <row r="78" spans="12:23">
-      <c r="L78" s="71"/>
-      <c r="M78" s="67"/>
-      <c r="N78" s="67"/>
-      <c r="O78" s="67"/>
-      <c r="P78" s="67"/>
-      <c r="Q78" s="67"/>
-      <c r="R78" s="67"/>
-      <c r="S78" s="67"/>
-      <c r="T78" s="67"/>
-      <c r="U78" s="67"/>
-      <c r="V78" s="67"/>
-      <c r="W78" s="67"/>
-    </row>
-    <row r="79" spans="12:23">
-      <c r="L79" s="71"/>
-      <c r="M79" s="67"/>
-      <c r="N79" s="67"/>
-      <c r="O79" s="67"/>
-      <c r="P79" s="67"/>
-      <c r="Q79" s="67"/>
-      <c r="R79" s="67"/>
-      <c r="S79" s="67"/>
-      <c r="T79" s="67"/>
-      <c r="U79" s="67"/>
-      <c r="V79" s="67"/>
-      <c r="W79" s="67"/>
-    </row>
-    <row r="80" spans="12:23">
-      <c r="L80" s="71"/>
-      <c r="M80" s="67"/>
-      <c r="N80" s="67"/>
-      <c r="O80" s="67"/>
-      <c r="P80" s="67"/>
-      <c r="Q80" s="67"/>
-      <c r="R80" s="67"/>
-      <c r="S80" s="67"/>
-      <c r="T80" s="67"/>
-      <c r="U80" s="67"/>
-      <c r="V80" s="67"/>
-      <c r="W80" s="67"/>
-    </row>
-    <row r="81" spans="12:23">
-      <c r="L81" s="71"/>
-      <c r="M81" s="67"/>
-      <c r="N81" s="67"/>
-      <c r="O81" s="67"/>
-      <c r="P81" s="67"/>
-      <c r="Q81" s="67"/>
-      <c r="R81" s="67"/>
-      <c r="S81" s="67"/>
-      <c r="T81" s="67"/>
-      <c r="U81" s="67"/>
-      <c r="V81" s="67"/>
-      <c r="W81" s="67"/>
-    </row>
-    <row r="82" spans="12:23">
-      <c r="L82" s="71"/>
-      <c r="M82" s="67"/>
-      <c r="N82" s="67"/>
-      <c r="O82" s="67"/>
-      <c r="P82" s="67"/>
-      <c r="Q82" s="67"/>
-      <c r="R82" s="67"/>
-      <c r="S82" s="67"/>
-      <c r="T82" s="67"/>
-      <c r="U82" s="67"/>
-      <c r="V82" s="67"/>
-      <c r="W82" s="67"/>
-    </row>
-    <row r="83" spans="12:23">
-      <c r="L83" s="71"/>
-      <c r="M83" s="67"/>
-      <c r="N83" s="67"/>
-      <c r="O83" s="67"/>
-      <c r="P83" s="67"/>
-      <c r="Q83" s="67"/>
-      <c r="R83" s="67"/>
-      <c r="S83" s="67"/>
-      <c r="T83" s="67"/>
-      <c r="U83" s="67"/>
-      <c r="V83" s="67"/>
-      <c r="W83" s="67"/>
-    </row>
-    <row r="84" spans="12:23">
-      <c r="L84" s="71"/>
-      <c r="M84" s="67"/>
-      <c r="N84" s="67"/>
-      <c r="O84" s="67"/>
-      <c r="P84" s="67"/>
-      <c r="Q84" s="67"/>
-      <c r="R84" s="67"/>
-      <c r="S84" s="67"/>
-      <c r="T84" s="67"/>
-      <c r="U84" s="67"/>
-      <c r="V84" s="67"/>
-      <c r="W84" s="67"/>
-    </row>
-    <row r="85" spans="12:23">
-      <c r="L85" s="71"/>
-      <c r="M85" s="67"/>
-      <c r="N85" s="67"/>
-      <c r="O85" s="67"/>
-      <c r="P85" s="67"/>
-      <c r="Q85" s="67"/>
-      <c r="R85" s="67"/>
-      <c r="S85" s="67"/>
-      <c r="T85" s="67"/>
-      <c r="U85" s="67"/>
-      <c r="V85" s="67"/>
-      <c r="W85" s="67"/>
-    </row>
-    <row r="86" spans="12:23">
-      <c r="L86" s="71"/>
-      <c r="M86" s="67"/>
-      <c r="N86" s="67"/>
-      <c r="O86" s="67"/>
-      <c r="P86" s="67"/>
-      <c r="Q86" s="67"/>
-      <c r="R86" s="67"/>
-      <c r="S86" s="67"/>
-      <c r="T86" s="67"/>
-      <c r="U86" s="67"/>
-      <c r="V86" s="67"/>
-      <c r="W86" s="67"/>
-    </row>
-    <row r="87" spans="12:23">
-      <c r="L87" s="71"/>
-      <c r="M87" s="67"/>
-      <c r="N87" s="67"/>
-      <c r="O87" s="67"/>
-      <c r="P87" s="67"/>
-      <c r="Q87" s="67"/>
-      <c r="R87" s="67"/>
-      <c r="S87" s="67"/>
-      <c r="T87" s="67"/>
-      <c r="U87" s="67"/>
-      <c r="V87" s="67"/>
-      <c r="W87" s="67"/>
-    </row>
-    <row r="88" spans="12:23">
-      <c r="L88" s="71"/>
-      <c r="M88" s="67"/>
-      <c r="N88" s="67"/>
-      <c r="O88" s="67"/>
-      <c r="P88" s="67"/>
-      <c r="Q88" s="67"/>
-      <c r="R88" s="67"/>
-      <c r="S88" s="67"/>
-      <c r="T88" s="67"/>
-      <c r="U88" s="67"/>
-      <c r="V88" s="67"/>
-      <c r="W88" s="67"/>
-    </row>
-    <row r="89" spans="12:23">
-      <c r="L89" s="71"/>
-      <c r="M89" s="67"/>
-      <c r="N89" s="67"/>
-      <c r="O89" s="67"/>
-      <c r="P89" s="67"/>
-      <c r="Q89" s="67"/>
-      <c r="R89" s="67"/>
-      <c r="S89" s="67"/>
-      <c r="T89" s="67"/>
-      <c r="U89" s="67"/>
-      <c r="V89" s="67"/>
-      <c r="W89" s="67"/>
-    </row>
-    <row r="90" spans="12:23">
-      <c r="L90" s="71"/>
-      <c r="M90" s="67"/>
-      <c r="N90" s="67"/>
-      <c r="O90" s="67"/>
-      <c r="P90" s="67"/>
-      <c r="Q90" s="67"/>
-      <c r="R90" s="67"/>
-      <c r="S90" s="67"/>
-      <c r="T90" s="67"/>
-      <c r="U90" s="67"/>
-      <c r="V90" s="67"/>
-      <c r="W90" s="67"/>
-    </row>
-    <row r="91" spans="12:23">
-      <c r="L91" s="71"/>
-      <c r="M91" s="67"/>
-      <c r="N91" s="67"/>
-      <c r="O91" s="67"/>
-      <c r="P91" s="67"/>
-      <c r="Q91" s="67"/>
-      <c r="R91" s="67"/>
-      <c r="S91" s="67"/>
-      <c r="T91" s="67"/>
-      <c r="U91" s="67"/>
-      <c r="V91" s="67"/>
-      <c r="W91" s="67"/>
-    </row>
-    <row r="92" spans="12:23">
-      <c r="L92" s="71"/>
-      <c r="M92" s="67"/>
-      <c r="N92" s="67"/>
-      <c r="O92" s="67"/>
-      <c r="P92" s="67"/>
-      <c r="Q92" s="67"/>
-      <c r="R92" s="67"/>
-      <c r="S92" s="67"/>
-      <c r="T92" s="67"/>
-      <c r="U92" s="67"/>
-      <c r="V92" s="67"/>
-      <c r="W92" s="67"/>
-    </row>
-    <row r="93" spans="12:23">
-      <c r="L93" s="71"/>
-      <c r="M93" s="67"/>
-      <c r="N93" s="67"/>
-      <c r="O93" s="67"/>
-      <c r="P93" s="67"/>
-      <c r="Q93" s="67"/>
-      <c r="R93" s="67"/>
-      <c r="S93" s="67"/>
-      <c r="T93" s="67"/>
-      <c r="U93" s="67"/>
-      <c r="V93" s="67"/>
-      <c r="W93" s="67"/>
-    </row>
-    <row r="94" spans="12:23">
-      <c r="L94" s="71"/>
-      <c r="M94" s="67"/>
-      <c r="N94" s="67"/>
-      <c r="O94" s="67"/>
-      <c r="P94" s="67"/>
-      <c r="Q94" s="67"/>
-      <c r="R94" s="67"/>
-      <c r="S94" s="67"/>
-      <c r="T94" s="67"/>
-      <c r="U94" s="67"/>
-      <c r="V94" s="67"/>
-      <c r="W94" s="67"/>
-    </row>
-    <row r="95" spans="12:23">
-      <c r="L95" s="71"/>
-      <c r="M95" s="67"/>
-      <c r="N95" s="67"/>
-      <c r="O95" s="67"/>
-      <c r="P95" s="67"/>
-      <c r="Q95" s="67"/>
-      <c r="R95" s="67"/>
-      <c r="S95" s="67"/>
-      <c r="T95" s="67"/>
-      <c r="U95" s="67"/>
-      <c r="V95" s="67"/>
-      <c r="W95" s="67"/>
-    </row>
-    <row r="96" spans="12:23">
-      <c r="L96" s="71"/>
-      <c r="M96" s="67"/>
-      <c r="N96" s="67"/>
-      <c r="O96" s="67"/>
-      <c r="P96" s="67"/>
-      <c r="Q96" s="67"/>
-      <c r="R96" s="67"/>
-      <c r="S96" s="67"/>
-      <c r="T96" s="67"/>
-      <c r="U96" s="67"/>
-      <c r="V96" s="67"/>
-      <c r="W96" s="67"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3"/>
+      <c r="T64" s="3"/>
+      <c r="U64" s="3"/>
+      <c r="V64" s="3"/>
+      <c r="W64" s="3"/>
+    </row>
+    <row r="65" spans="13:23">
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+      <c r="V65" s="3"/>
+      <c r="W65" s="3"/>
+    </row>
+    <row r="66" spans="13:23">
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+      <c r="U66" s="3"/>
+      <c r="V66" s="3"/>
+      <c r="W66" s="3"/>
+    </row>
+    <row r="67" spans="13:23">
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+      <c r="V67" s="3"/>
+      <c r="W67" s="3"/>
+    </row>
+    <row r="68" spans="13:23">
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
+    </row>
+    <row r="69" spans="13:23">
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="3"/>
+      <c r="T69" s="3"/>
+      <c r="U69" s="3"/>
+      <c r="V69" s="3"/>
+      <c r="W69" s="3"/>
+    </row>
+    <row r="70" spans="13:23">
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+      <c r="V70" s="3"/>
+      <c r="W70" s="3"/>
+    </row>
+    <row r="71" spans="13:23">
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="U71" s="3"/>
+      <c r="V71" s="3"/>
+      <c r="W71" s="3"/>
+    </row>
+    <row r="72" spans="13:23">
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="3"/>
+      <c r="T72" s="3"/>
+      <c r="U72" s="3"/>
+      <c r="V72" s="3"/>
+      <c r="W72" s="3"/>
+    </row>
+    <row r="73" spans="13:23">
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="3"/>
+      <c r="T73" s="3"/>
+      <c r="U73" s="3"/>
+      <c r="V73" s="3"/>
+      <c r="W73" s="3"/>
+    </row>
+    <row r="74" spans="13:23">
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+      <c r="P74" s="3"/>
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="3"/>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
+      <c r="W74" s="3"/>
+    </row>
+    <row r="75" spans="13:23">
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="3"/>
+      <c r="T75" s="3"/>
+      <c r="U75" s="3"/>
+      <c r="V75" s="3"/>
+      <c r="W75" s="3"/>
+    </row>
+    <row r="76" spans="13:23">
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3"/>
+      <c r="S76" s="3"/>
+      <c r="T76" s="3"/>
+      <c r="U76" s="3"/>
+      <c r="V76" s="3"/>
+      <c r="W76" s="3"/>
+    </row>
+    <row r="77" spans="13:23">
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+      <c r="Q77" s="3"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="3"/>
+      <c r="T77" s="3"/>
+      <c r="U77" s="3"/>
+      <c r="V77" s="3"/>
+      <c r="W77" s="3"/>
+    </row>
+    <row r="78" spans="13:23">
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3"/>
+      <c r="V78" s="3"/>
+      <c r="W78" s="3"/>
+    </row>
+    <row r="79" spans="13:23">
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3"/>
+      <c r="T79" s="3"/>
+      <c r="U79" s="3"/>
+      <c r="V79" s="3"/>
+      <c r="W79" s="3"/>
+    </row>
+    <row r="80" spans="13:23">
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="3"/>
+      <c r="T80" s="3"/>
+      <c r="U80" s="3"/>
+      <c r="V80" s="3"/>
+      <c r="W80" s="3"/>
+    </row>
+    <row r="81" spans="13:23">
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="3"/>
+      <c r="T81" s="3"/>
+      <c r="U81" s="3"/>
+      <c r="V81" s="3"/>
+      <c r="W81" s="3"/>
+    </row>
+    <row r="82" spans="13:23">
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3"/>
+      <c r="Q82" s="3"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="3"/>
+      <c r="T82" s="3"/>
+      <c r="U82" s="3"/>
+      <c r="V82" s="3"/>
+      <c r="W82" s="3"/>
+    </row>
+    <row r="83" spans="13:23">
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
+      <c r="Q83" s="3"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="3"/>
+      <c r="T83" s="3"/>
+      <c r="U83" s="3"/>
+      <c r="V83" s="3"/>
+      <c r="W83" s="3"/>
+    </row>
+    <row r="84" spans="13:23">
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="3"/>
+      <c r="P84" s="3"/>
+      <c r="Q84" s="3"/>
+      <c r="R84" s="3"/>
+      <c r="S84" s="3"/>
+      <c r="T84" s="3"/>
+      <c r="U84" s="3"/>
+      <c r="V84" s="3"/>
+      <c r="W84" s="3"/>
+    </row>
+    <row r="85" spans="13:23">
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="3"/>
+      <c r="T85" s="3"/>
+      <c r="U85" s="3"/>
+      <c r="V85" s="3"/>
+      <c r="W85" s="3"/>
+    </row>
+    <row r="86" spans="13:23">
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="3"/>
+      <c r="T86" s="3"/>
+      <c r="U86" s="3"/>
+      <c r="V86" s="3"/>
+      <c r="W86" s="3"/>
+    </row>
+    <row r="87" spans="13:23">
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="3"/>
+      <c r="T87" s="3"/>
+      <c r="U87" s="3"/>
+      <c r="V87" s="3"/>
+      <c r="W87" s="3"/>
+    </row>
+    <row r="88" spans="13:23">
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="3"/>
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="3"/>
+      <c r="T88" s="3"/>
+      <c r="U88" s="3"/>
+      <c r="V88" s="3"/>
+      <c r="W88" s="3"/>
+    </row>
+    <row r="89" spans="13:23">
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
+      <c r="Q89" s="3"/>
+      <c r="R89" s="3"/>
+      <c r="S89" s="3"/>
+      <c r="T89" s="3"/>
+      <c r="U89" s="3"/>
+      <c r="V89" s="3"/>
+      <c r="W89" s="3"/>
+    </row>
+    <row r="90" spans="13:23">
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
+    </row>
+    <row r="91" spans="13:23">
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="3"/>
+      <c r="T91" s="3"/>
+      <c r="U91" s="3"/>
+      <c r="V91" s="3"/>
+      <c r="W91" s="3"/>
+    </row>
+    <row r="92" spans="13:23">
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="3"/>
+      <c r="T92" s="3"/>
+      <c r="U92" s="3"/>
+      <c r="V92" s="3"/>
+      <c r="W92" s="3"/>
+    </row>
+    <row r="93" spans="13:23">
+      <c r="M93" s="3"/>
+      <c r="N93" s="3"/>
+      <c r="O93" s="3"/>
+      <c r="P93" s="3"/>
+      <c r="Q93" s="3"/>
+      <c r="R93" s="3"/>
+      <c r="S93" s="3"/>
+      <c r="T93" s="3"/>
+      <c r="U93" s="3"/>
+      <c r="V93" s="3"/>
+      <c r="W93" s="3"/>
+    </row>
+    <row r="94" spans="13:23">
+      <c r="M94" s="3"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="3"/>
+      <c r="P94" s="3"/>
+      <c r="Q94" s="3"/>
+      <c r="R94" s="3"/>
+      <c r="S94" s="3"/>
+      <c r="T94" s="3"/>
+      <c r="U94" s="3"/>
+      <c r="V94" s="3"/>
+      <c r="W94" s="3"/>
+    </row>
+    <row r="95" spans="13:23">
+      <c r="M95" s="3"/>
+      <c r="N95" s="3"/>
+      <c r="O95" s="3"/>
+      <c r="P95" s="3"/>
+      <c r="Q95" s="3"/>
+      <c r="R95" s="3"/>
+      <c r="S95" s="3"/>
+      <c r="T95" s="3"/>
+      <c r="U95" s="3"/>
+      <c r="V95" s="3"/>
+      <c r="W95" s="3"/>
+    </row>
+    <row r="96" spans="13:23">
+      <c r="M96" s="3"/>
+      <c r="N96" s="3"/>
+      <c r="O96" s="3"/>
+      <c r="P96" s="3"/>
+      <c r="Q96" s="3"/>
+      <c r="R96" s="3"/>
+      <c r="S96" s="3"/>
+      <c r="T96" s="3"/>
+      <c r="U96" s="3"/>
+      <c r="V96" s="3"/>
+      <c r="W96" s="3"/>
     </row>
     <row r="102" spans="10:21">
       <c r="J102" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="104" spans="10:21">
       <c r="K104" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="106" spans="10:21">
       <c r="K106" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="108" spans="10:21">
       <c r="K108" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="111" spans="10:21">
       <c r="K111" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="U111" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="U111" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="126" spans="10:10">
+    </row>
+    <row r="126" spans="10:11">
       <c r="J126" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="128" spans="10:11">
+      <c r="K128" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="130" spans="11:11">
+      <c r="K130" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="132" spans="11:11">
+      <c r="K132" s="1" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="140" spans="9:10">
-      <c r="I140" s="8" t="s">
+    <row r="153" spans="10:10">
+      <c r="J153" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="155" spans="10:10">
+      <c r="J155" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="188" spans="9:10">
+      <c r="I188" s="8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="190" spans="9:10">
+      <c r="J190" s="1" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="142" spans="9:10">
-      <c r="J142" s="1" t="s">
+    <row r="192" spans="9:10">
+      <c r="J192" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="193" spans="11:30">
+      <c r="K193" s="1" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="144" spans="9:10">
-      <c r="J144" s="2" t="s">
+      <c r="AD193" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="213" spans="10:30">
+      <c r="J213" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="216" spans="10:30">
+      <c r="K216" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="AD216" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="237" spans="14:35">
+      <c r="N237" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="X237" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="145" spans="11:30">
-      <c r="K145" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="AD145" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="165" spans="10:30">
-      <c r="J165" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="168" spans="10:30">
-      <c r="K168" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="AD168" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="189" spans="14:35">
-      <c r="N189" s="1" t="s">
+      <c r="AI237" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="238" spans="14:35">
+      <c r="X238" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="X189" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI189" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="190" spans="14:35">
-      <c r="X190" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="199" spans="29:29">
-      <c r="AC199" s="3"/>
+    </row>
+    <row r="247" spans="29:29">
+      <c r="AC247" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -39900,12 +40453,12 @@
     <mergeCell ref="U61:W61"/>
     <mergeCell ref="U60:W60"/>
     <mergeCell ref="O57:T57"/>
+    <mergeCell ref="M61:N61"/>
     <mergeCell ref="L57:L59"/>
     <mergeCell ref="M57:N57"/>
     <mergeCell ref="M58:N58"/>
     <mergeCell ref="M59:N59"/>
     <mergeCell ref="M60:N60"/>
-    <mergeCell ref="M61:N61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39928,7 +40481,7 @@
   <sheetData>
     <row r="4" spans="3:8">
       <c r="C4" s="53" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D4" s="53"/>
       <c r="E4" s="53"/>
@@ -39947,7 +40500,7 @@
     <row r="6" spans="3:8">
       <c r="C6" s="53"/>
       <c r="D6" s="53" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E6" s="53"/>
       <c r="F6" s="53"/>
@@ -39990,7 +40543,7 @@
     </row>
     <row r="7" spans="3:17">
       <c r="C7" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D7" s="53"/>
       <c r="E7" s="53"/>
@@ -40025,7 +40578,7 @@
     <row r="9" spans="3:17">
       <c r="C9" s="53"/>
       <c r="D9" s="53" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E9" s="53"/>
       <c r="F9" s="53"/>
@@ -40060,7 +40613,7 @@
       <c r="C11" s="53"/>
       <c r="D11" s="53"/>
       <c r="E11" s="53" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F11" s="53"/>
       <c r="G11" s="53"/>
@@ -40094,7 +40647,7 @@
       <c r="C13" s="53"/>
       <c r="D13" s="53"/>
       <c r="E13" s="53" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F13" s="53"/>
       <c r="G13" s="53"/>
@@ -40125,7 +40678,7 @@
     <row r="15" spans="3:17">
       <c r="C15" s="53"/>
       <c r="D15" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E15" s="53"/>
       <c r="F15" s="53"/>
@@ -40155,7 +40708,7 @@
     <row r="17" spans="3:14">
       <c r="C17" s="53"/>
       <c r="D17" s="53" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E17" s="53"/>
       <c r="F17" s="53"/>

</xml_diff>